<commit_message>
update with final parameter-change-experiment
</commit_message>
<xml_diff>
--- a/PycharmCodes_xlsxFiles/parameter_to_force/parameter_to_force_n.xlsx
+++ b/PycharmCodes_xlsxFiles/parameter_to_force/parameter_to_force_n.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7d89e7b822021c56/Documents/성균관대학교/LAB/skku_robotory/PycharmCodes_xlsxFiles/parameter_to_force/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="8_{2795DAF1-47A8-4C0A-B1C8-7E8923DBA3A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D32B3A15-CDFC-4ADF-94B8-058B087B1C78}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="8_{2795DAF1-47A8-4C0A-B1C8-7E8923DBA3A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{034DF233-6816-430E-B275-D336047D2FA6}"/>
   <bookViews>
-    <workbookView xWindow="6972" yWindow="1608" windowWidth="17280" windowHeight="8880" activeTab="3" xr2:uid="{931566E5-BD05-4787-8A70-E08F34399E6B}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="3" xr2:uid="{931566E5-BD05-4787-8A70-E08F34399E6B}"/>
   </bookViews>
   <sheets>
     <sheet name="dn" sheetId="1" r:id="rId1"/>
@@ -134,7 +134,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,26 +168,11 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="7" tint="0.39997558519241921"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
     </font>
     <font>
       <sz val="11"/>
@@ -218,9 +203,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -233,13 +218,26 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -256,6 +254,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -577,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5988321D-DF54-400E-9133-239544CD0B21}">
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -638,170 +640,290 @@
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
+      <c r="B2" s="4">
+        <v>0.91</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.98</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.63</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1.49</v>
+      </c>
+      <c r="F2" s="4">
+        <v>1.58</v>
+      </c>
+      <c r="G2" s="4">
+        <v>1.29</v>
+      </c>
+      <c r="H2" s="4">
+        <v>1.93</v>
+      </c>
+      <c r="I2" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="J2" s="4">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="K2" s="4">
+        <v>2.62</v>
+      </c>
+      <c r="L2" s="4">
+        <v>2.71</v>
+      </c>
+      <c r="M2" s="4">
+        <v>2.78</v>
+      </c>
+      <c r="N2" s="4">
+        <v>3.26</v>
+      </c>
+      <c r="O2" s="4">
+        <v>3.31</v>
+      </c>
+      <c r="P2" s="4">
+        <v>3.4</v>
+      </c>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
+      <c r="B3" s="4">
+        <v>1.75</v>
+      </c>
+      <c r="C3" s="4">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4">
+        <v>2.15</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2.68</v>
+      </c>
+      <c r="F3" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="G3" s="4">
+        <v>3.02</v>
+      </c>
+      <c r="H3" s="4">
+        <v>3.62</v>
+      </c>
+      <c r="I3" s="4">
+        <v>3.78</v>
+      </c>
+      <c r="J3" s="4">
+        <v>3.89</v>
+      </c>
+      <c r="K3" s="4">
+        <v>4.54</v>
+      </c>
+      <c r="L3" s="4">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="M3" s="4">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="N3" s="4">
+        <v>5.34</v>
+      </c>
+      <c r="O3" s="4">
+        <v>5.2</v>
+      </c>
+      <c r="P3" s="4">
+        <v>5.35</v>
+      </c>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
+      <c r="B4" s="4">
+        <v>1.89</v>
+      </c>
+      <c r="C4" s="4">
+        <v>2.16</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2.92</v>
+      </c>
+      <c r="F4" s="4">
+        <v>3.03</v>
+      </c>
+      <c r="G4" s="4">
+        <v>2.9</v>
+      </c>
+      <c r="H4" s="4">
+        <v>3.94</v>
+      </c>
+      <c r="I4" s="4">
+        <v>4.07</v>
+      </c>
+      <c r="J4" s="4">
+        <v>4.09</v>
+      </c>
+      <c r="K4" s="4">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="L4" s="4">
+        <v>4.97</v>
+      </c>
+      <c r="M4" s="4">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="N4" s="4">
+        <v>5.47</v>
+      </c>
+      <c r="O4" s="4">
+        <v>5.49</v>
+      </c>
+      <c r="P4" s="4">
+        <v>5.79</v>
+      </c>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
+      <c r="B5" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1.34</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="E5" s="4">
+        <v>2.44</v>
+      </c>
+      <c r="F5" s="4">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="G5" s="4">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="H5" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="I5" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="J5" s="4">
+        <v>3.12</v>
+      </c>
+      <c r="K5" s="4">
+        <v>4.12</v>
+      </c>
+      <c r="L5" s="4">
+        <v>4.12</v>
+      </c>
+      <c r="M5" s="4">
+        <v>4.18</v>
+      </c>
+      <c r="N5" s="4">
+        <v>4.88</v>
+      </c>
+      <c r="O5" s="4">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="P5" s="4">
+        <v>5.12</v>
+      </c>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="6">
-        <v>0.96</v>
-      </c>
-      <c r="C6" s="6">
-        <v>0.98</v>
-      </c>
-      <c r="D6" s="6">
-        <v>1</v>
-      </c>
-      <c r="E6" s="6">
-        <v>1.96</v>
-      </c>
-      <c r="F6" s="6">
-        <v>1.94</v>
-      </c>
-      <c r="G6" s="6">
-        <v>1.94</v>
-      </c>
-      <c r="H6" s="6">
-        <v>2.79</v>
-      </c>
-      <c r="I6" s="6">
-        <v>2.76</v>
-      </c>
-      <c r="J6" s="6">
-        <v>2.81</v>
-      </c>
-      <c r="K6" s="6">
-        <v>3.59</v>
-      </c>
-      <c r="L6" s="6">
-        <v>3.54</v>
-      </c>
-      <c r="M6" s="6">
-        <v>3.53</v>
-      </c>
-      <c r="N6" s="6">
-        <v>4.21</v>
-      </c>
-      <c r="O6" s="6">
-        <v>4.1399999999999997</v>
-      </c>
-      <c r="P6" s="6">
-        <v>4.01</v>
-      </c>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
+      <c r="B6" s="4">
+        <v>1.25</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1.27</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1.31</v>
+      </c>
+      <c r="E6" s="4">
+        <v>2.52</v>
+      </c>
+      <c r="F6" s="4">
+        <v>2.52</v>
+      </c>
+      <c r="G6" s="4">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="H6" s="4">
+        <v>3.65</v>
+      </c>
+      <c r="I6" s="4">
+        <v>3.67</v>
+      </c>
+      <c r="J6" s="4">
+        <v>3.69</v>
+      </c>
+      <c r="K6" s="4">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="L6" s="4">
+        <v>4.71</v>
+      </c>
+      <c r="M6" s="4">
+        <v>4.74</v>
+      </c>
+      <c r="N6" s="4">
+        <v>5.61</v>
+      </c>
+      <c r="O6" s="4">
+        <v>5.66</v>
+      </c>
+      <c r="P6" s="4">
+        <v>5.69</v>
+      </c>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A7" s="1"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A8" s="1"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -813,8 +935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB40293F-A8B5-4003-A866-76DFC9ACBB39}">
   <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:V6"/>
+    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -888,88 +1010,340 @@
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="B2" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1.22</v>
+      </c>
+      <c r="D2" s="5">
+        <v>1.27</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1.43</v>
+      </c>
+      <c r="F2" s="6">
+        <v>1.88</v>
+      </c>
+      <c r="G2" s="6">
+        <v>1.95</v>
+      </c>
+      <c r="H2" s="7">
+        <v>2.15</v>
+      </c>
+      <c r="I2" s="7">
+        <v>2.66</v>
+      </c>
+      <c r="J2" s="7">
+        <v>2.77</v>
+      </c>
+      <c r="K2" s="8">
+        <v>3.35</v>
+      </c>
+      <c r="L2" s="8">
+        <v>3.76</v>
+      </c>
+      <c r="M2" s="8">
+        <v>3.82</v>
+      </c>
+      <c r="N2" s="9">
+        <v>4.78</v>
+      </c>
+      <c r="O2" s="9">
+        <v>4.91</v>
+      </c>
+      <c r="P2" s="9">
+        <v>5.03</v>
+      </c>
+      <c r="Q2" s="10">
+        <v>6.33</v>
+      </c>
+      <c r="R2" s="10">
+        <v>6.36</v>
+      </c>
+      <c r="S2" s="10">
+        <v>6.36</v>
+      </c>
+      <c r="T2" s="11">
+        <v>7.92</v>
+      </c>
+      <c r="U2" s="11">
+        <v>7.91</v>
+      </c>
+      <c r="V2" s="11">
+        <v>7.95</v>
+      </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="B3" s="5">
+        <v>0.85</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.16</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.24</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1.83</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0.87</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0.79</v>
+      </c>
+      <c r="H3" s="7">
+        <v>2.93</v>
+      </c>
+      <c r="I3" s="7">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="J3" s="7">
+        <v>2.21</v>
+      </c>
+      <c r="K3" s="8">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="L3" s="8">
+        <v>4.24</v>
+      </c>
+      <c r="M3" s="8">
+        <v>4.03</v>
+      </c>
+      <c r="N3" s="9">
+        <v>6.18</v>
+      </c>
+      <c r="O3" s="9">
+        <v>5.99</v>
+      </c>
+      <c r="P3" s="9">
+        <v>5.98</v>
+      </c>
+      <c r="Q3" s="10">
+        <v>8.07</v>
+      </c>
+      <c r="R3" s="10">
+        <v>8.11</v>
+      </c>
+      <c r="S3" s="10">
+        <v>8.14</v>
+      </c>
+      <c r="T3" s="11">
+        <v>10.4</v>
+      </c>
+      <c r="U3" s="11">
+        <v>10.28</v>
+      </c>
+      <c r="V3" s="11">
+        <v>10.26</v>
+      </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="B4" s="5">
+        <v>1.25</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1.42</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1.08</v>
+      </c>
+      <c r="E4" s="6">
+        <v>2.54</v>
+      </c>
+      <c r="F4" s="6">
+        <v>2.77</v>
+      </c>
+      <c r="G4" s="6">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="H4" s="7">
+        <v>4.18</v>
+      </c>
+      <c r="I4" s="7">
+        <v>4.33</v>
+      </c>
+      <c r="J4" s="7">
+        <v>4.09</v>
+      </c>
+      <c r="K4" s="8">
+        <v>6.42</v>
+      </c>
+      <c r="L4" s="8">
+        <v>6.33</v>
+      </c>
+      <c r="M4" s="8">
+        <v>6.28</v>
+      </c>
+      <c r="N4" s="9">
+        <v>8.35</v>
+      </c>
+      <c r="O4" s="9">
+        <v>8.36</v>
+      </c>
+      <c r="P4" s="9">
+        <v>8.57</v>
+      </c>
+      <c r="Q4" s="10">
+        <v>10.84</v>
+      </c>
+      <c r="R4" s="10">
+        <v>10.85</v>
+      </c>
+      <c r="S4" s="10">
+        <v>10.94</v>
+      </c>
+      <c r="T4" s="11">
+        <v>13.23</v>
+      </c>
+      <c r="U4" s="11">
+        <v>13.24</v>
+      </c>
+      <c r="V4" s="11">
+        <v>13.21</v>
+      </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="B5" s="5">
+        <v>1.59</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1.31</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1.29</v>
+      </c>
+      <c r="E5" s="6">
+        <v>3.59</v>
+      </c>
+      <c r="F5" s="6">
+        <v>3.51</v>
+      </c>
+      <c r="G5" s="6">
+        <v>3.47</v>
+      </c>
+      <c r="H5" s="7">
+        <v>5.87</v>
+      </c>
+      <c r="I5" s="7">
+        <v>5.91</v>
+      </c>
+      <c r="J5" s="7">
+        <v>5.81</v>
+      </c>
+      <c r="K5" s="8">
+        <v>8.2799999999999994</v>
+      </c>
+      <c r="L5" s="8">
+        <v>8.36</v>
+      </c>
+      <c r="M5" s="8">
+        <v>8.3800000000000008</v>
+      </c>
+      <c r="N5" s="9">
+        <v>10.72</v>
+      </c>
+      <c r="O5" s="9">
+        <v>10.72</v>
+      </c>
+      <c r="P5" s="9">
+        <v>10.74</v>
+      </c>
+      <c r="Q5" s="10">
+        <v>13.14</v>
+      </c>
+      <c r="R5" s="10">
+        <v>13.07</v>
+      </c>
+      <c r="S5" s="10">
+        <v>12.93</v>
+      </c>
+      <c r="T5" s="11">
+        <v>15.62</v>
+      </c>
+      <c r="U5" s="11">
+        <v>15.62</v>
+      </c>
+      <c r="V5" s="11">
+        <v>15.18</v>
+      </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="6">
-        <v>2.4500000000000002</v>
-      </c>
-      <c r="C6" s="6">
-        <v>2.33</v>
-      </c>
-      <c r="D6" s="6">
-        <v>2.33</v>
+      <c r="B6" s="5">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2.35</v>
+      </c>
+      <c r="D6" s="5">
+        <v>2.37</v>
       </c>
       <c r="E6" s="6">
-        <v>4.84</v>
+        <v>4.6900000000000004</v>
       </c>
       <c r="F6" s="6">
-        <v>4.63</v>
+        <v>4.6900000000000004</v>
       </c>
       <c r="G6" s="6">
         <v>4.62</v>
       </c>
-      <c r="H6" s="6">
-        <v>7.19</v>
-      </c>
-      <c r="I6" s="6">
-        <v>7</v>
-      </c>
-      <c r="J6" s="6">
-        <v>6.97</v>
-      </c>
-      <c r="K6" s="6">
-        <v>9.61</v>
-      </c>
-      <c r="L6" s="6">
-        <v>9.41</v>
-      </c>
-      <c r="M6" s="6">
-        <v>9.3699999999999992</v>
-      </c>
-      <c r="N6" s="6">
-        <v>12.24</v>
-      </c>
-      <c r="O6" s="6">
-        <v>11.85</v>
-      </c>
-      <c r="P6" s="6">
-        <v>11.83</v>
-      </c>
-      <c r="Q6" s="6">
-        <v>14.71</v>
-      </c>
-      <c r="R6" s="6">
-        <v>14.33</v>
-      </c>
-      <c r="S6" s="6">
-        <v>14.17</v>
-      </c>
-      <c r="T6" s="6">
-        <v>17.170000000000002</v>
-      </c>
-      <c r="U6" s="6">
-        <v>16.73</v>
-      </c>
-      <c r="V6" s="6">
-        <v>16.66</v>
+      <c r="H6" s="7">
+        <v>7.09</v>
+      </c>
+      <c r="I6" s="7">
+        <v>6.93</v>
+      </c>
+      <c r="J6" s="7">
+        <v>6.92</v>
+      </c>
+      <c r="K6" s="8">
+        <v>9.52</v>
+      </c>
+      <c r="L6" s="8">
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="M6" s="8">
+        <v>9.26</v>
+      </c>
+      <c r="N6" s="9">
+        <v>11.88</v>
+      </c>
+      <c r="O6" s="9">
+        <v>11.6</v>
+      </c>
+      <c r="P6" s="9">
+        <v>11.59</v>
+      </c>
+      <c r="Q6" s="10">
+        <v>14.01</v>
+      </c>
+      <c r="R6" s="10">
+        <v>13.94</v>
+      </c>
+      <c r="S6" s="10">
+        <v>13.87</v>
+      </c>
+      <c r="T6" s="11">
+        <v>16.37</v>
+      </c>
+      <c r="U6" s="11">
+        <v>16.23</v>
+      </c>
+      <c r="V6" s="11">
+        <v>16.149999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -982,8 +1356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3069BDF-C53E-4752-A5CB-A4AF697C25ED}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:P6"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1039,70 +1413,250 @@
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="B2" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="C2" s="12">
+        <v>0.17</v>
+      </c>
+      <c r="D2" s="12">
+        <v>0.17</v>
+      </c>
+      <c r="E2" s="13">
+        <v>0.72</v>
+      </c>
+      <c r="F2" s="13">
+        <v>0.68</v>
+      </c>
+      <c r="G2" s="13">
+        <v>0.65</v>
+      </c>
+      <c r="H2" s="14">
+        <v>1.62</v>
+      </c>
+      <c r="I2" s="14">
+        <v>1.58</v>
+      </c>
+      <c r="J2" s="14">
+        <v>1.58</v>
+      </c>
+      <c r="K2" s="15">
+        <v>2.52</v>
+      </c>
+      <c r="L2" s="15">
+        <v>2.48</v>
+      </c>
+      <c r="M2" s="15">
+        <v>2.48</v>
+      </c>
+      <c r="N2" s="16">
+        <v>3.38</v>
+      </c>
+      <c r="O2" s="16">
+        <v>3.02</v>
+      </c>
+      <c r="P2" s="16">
+        <v>3.14</v>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="B3" s="12">
+        <v>0.21</v>
+      </c>
+      <c r="C3" s="12">
+        <v>0.19</v>
+      </c>
+      <c r="D3" s="12">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E3" s="13">
+        <v>1.38</v>
+      </c>
+      <c r="F3" s="13">
+        <v>1.35</v>
+      </c>
+      <c r="G3" s="13">
+        <v>1.35</v>
+      </c>
+      <c r="H3" s="14">
+        <v>2.54</v>
+      </c>
+      <c r="I3" s="14">
+        <v>2.64</v>
+      </c>
+      <c r="J3" s="14">
+        <v>2.64</v>
+      </c>
+      <c r="K3" s="15">
+        <v>3.84</v>
+      </c>
+      <c r="L3" s="15">
+        <v>3.85</v>
+      </c>
+      <c r="M3" s="15">
+        <v>3.86</v>
+      </c>
+      <c r="N3" s="16">
+        <v>4.84</v>
+      </c>
+      <c r="O3" s="16">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="P3" s="16">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="B4" s="12">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C4" s="12">
+        <v>0.49</v>
+      </c>
+      <c r="D4" s="12">
+        <v>0.45</v>
+      </c>
+      <c r="E4" s="13">
+        <v>1.46</v>
+      </c>
+      <c r="F4" s="13">
+        <v>1.47</v>
+      </c>
+      <c r="G4" s="13">
+        <v>1.43</v>
+      </c>
+      <c r="H4" s="14">
+        <v>2.65</v>
+      </c>
+      <c r="I4" s="14">
+        <v>2.68</v>
+      </c>
+      <c r="J4" s="14">
+        <v>2.5</v>
+      </c>
+      <c r="K4" s="15">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="L4" s="15">
+        <v>4.04</v>
+      </c>
+      <c r="M4" s="15">
+        <v>3.98</v>
+      </c>
+      <c r="N4" s="16">
+        <v>5.65</v>
+      </c>
+      <c r="O4" s="16">
+        <v>5.33</v>
+      </c>
+      <c r="P4" s="16">
+        <v>5.19</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="B5" s="12">
+        <v>0.44</v>
+      </c>
+      <c r="C5" s="12">
+        <v>0.39</v>
+      </c>
+      <c r="D5" s="12">
+        <v>0.38</v>
+      </c>
+      <c r="E5" s="13">
+        <v>2.1</v>
+      </c>
+      <c r="F5" s="13">
+        <v>2.14</v>
+      </c>
+      <c r="G5" s="13">
+        <v>2.04</v>
+      </c>
+      <c r="H5" s="14">
+        <v>3.84</v>
+      </c>
+      <c r="I5" s="14">
+        <v>3.85</v>
+      </c>
+      <c r="J5" s="14">
+        <v>3.88</v>
+      </c>
+      <c r="K5" s="15">
+        <v>5.33</v>
+      </c>
+      <c r="L5" s="15">
+        <v>5.38</v>
+      </c>
+      <c r="M5" s="15">
+        <v>5.35</v>
+      </c>
+      <c r="N5" s="16">
+        <v>6.6</v>
+      </c>
+      <c r="O5" s="16">
+        <v>6.9</v>
+      </c>
+      <c r="P5" s="16">
+        <v>6.85</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="6">
-        <v>1.31</v>
-      </c>
-      <c r="C6" s="6">
-        <v>1.53</v>
-      </c>
-      <c r="D6" s="6">
-        <v>1.56</v>
-      </c>
-      <c r="E6" s="6">
-        <v>2.95</v>
-      </c>
-      <c r="F6" s="6">
-        <v>3.06</v>
-      </c>
-      <c r="G6" s="6">
-        <v>3.08</v>
-      </c>
-      <c r="H6" s="6">
-        <v>4.62</v>
-      </c>
-      <c r="I6" s="6">
-        <v>4.63</v>
-      </c>
-      <c r="J6" s="6">
-        <v>4.66</v>
-      </c>
-      <c r="K6" s="6">
-        <v>6.18</v>
-      </c>
-      <c r="L6" s="6">
-        <v>6.2</v>
-      </c>
-      <c r="M6" s="6">
-        <v>6.2</v>
-      </c>
-      <c r="N6" s="6">
-        <v>7.66</v>
-      </c>
-      <c r="O6" s="6">
-        <v>7.68</v>
-      </c>
-      <c r="P6" s="6">
-        <v>7.4</v>
+      <c r="B6" s="12">
+        <v>0.88</v>
+      </c>
+      <c r="C6" s="12">
+        <v>0.88</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0.73</v>
+      </c>
+      <c r="E6" s="13">
+        <v>1.77</v>
+      </c>
+      <c r="F6" s="13">
+        <v>1.94</v>
+      </c>
+      <c r="G6" s="13">
+        <v>2.11</v>
+      </c>
+      <c r="H6" s="14">
+        <v>3.31</v>
+      </c>
+      <c r="I6" s="14">
+        <v>3.54</v>
+      </c>
+      <c r="J6" s="14">
+        <v>3.78</v>
+      </c>
+      <c r="K6" s="15">
+        <v>4.72</v>
+      </c>
+      <c r="L6" s="15">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="M6" s="15">
+        <v>5.32</v>
+      </c>
+      <c r="N6" s="16">
+        <v>6.22</v>
+      </c>
+      <c r="O6" s="16">
+        <v>6.39</v>
+      </c>
+      <c r="P6" s="16">
+        <v>6.81</v>
       </c>
     </row>
   </sheetData>
@@ -1115,8 +1669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00ECCB68-6F4A-4958-940C-64784FBE056C}">
   <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2:V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1190,88 +1744,340 @@
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="B2" s="17">
+        <v>0.11</v>
+      </c>
+      <c r="C2" s="17">
+        <v>0.12</v>
+      </c>
+      <c r="D2" s="17">
+        <v>0.18</v>
+      </c>
+      <c r="E2" s="18">
+        <v>0.24</v>
+      </c>
+      <c r="F2" s="18">
+        <v>0.27</v>
+      </c>
+      <c r="G2" s="18">
+        <v>0.3</v>
+      </c>
+      <c r="H2" s="19">
+        <v>0.41</v>
+      </c>
+      <c r="I2" s="19">
+        <v>0.43</v>
+      </c>
+      <c r="J2" s="19">
+        <v>0.46</v>
+      </c>
+      <c r="K2" s="20">
+        <v>0.61</v>
+      </c>
+      <c r="L2" s="20">
+        <v>0.64</v>
+      </c>
+      <c r="M2" s="20">
+        <v>0.65</v>
+      </c>
+      <c r="N2" s="21">
+        <v>0.74</v>
+      </c>
+      <c r="O2" s="21">
+        <v>0.74</v>
+      </c>
+      <c r="P2" s="21">
+        <v>0.74</v>
+      </c>
+      <c r="Q2" s="22">
+        <v>0.97</v>
+      </c>
+      <c r="R2" s="22">
+        <v>0.98</v>
+      </c>
+      <c r="S2" s="22">
+        <v>1</v>
+      </c>
+      <c r="T2" s="23">
+        <v>1.26</v>
+      </c>
+      <c r="U2" s="23">
+        <v>1.24</v>
+      </c>
+      <c r="V2" s="23">
+        <v>1.23</v>
+      </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="B3" s="17">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C3" s="17">
+        <v>0.32</v>
+      </c>
+      <c r="D3" s="17">
+        <v>0.4</v>
+      </c>
+      <c r="E3" s="18">
+        <v>1</v>
+      </c>
+      <c r="F3" s="18">
+        <v>0.84</v>
+      </c>
+      <c r="G3" s="18">
+        <v>0.76</v>
+      </c>
+      <c r="H3" s="19">
+        <v>1.45</v>
+      </c>
+      <c r="I3" s="19">
+        <v>1.28</v>
+      </c>
+      <c r="J3" s="19">
+        <v>1.21</v>
+      </c>
+      <c r="K3" s="20">
+        <v>1.89</v>
+      </c>
+      <c r="L3" s="20">
+        <v>1.74</v>
+      </c>
+      <c r="M3" s="20">
+        <v>1.66</v>
+      </c>
+      <c r="N3" s="21">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="O3" s="21">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="P3" s="21">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="Q3" s="22">
+        <v>2.65</v>
+      </c>
+      <c r="R3" s="22">
+        <v>2.58</v>
+      </c>
+      <c r="S3" s="22">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="T3" s="23">
+        <v>3.21</v>
+      </c>
+      <c r="U3" s="23">
+        <v>3.12</v>
+      </c>
+      <c r="V3" s="23">
+        <v>3.05</v>
+      </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="B4" s="17">
+        <v>0.79</v>
+      </c>
+      <c r="C4" s="17">
+        <v>0.68</v>
+      </c>
+      <c r="D4" s="17">
+        <v>0.89</v>
+      </c>
+      <c r="E4" s="18">
+        <v>1.3</v>
+      </c>
+      <c r="F4" s="18">
+        <v>1.38</v>
+      </c>
+      <c r="G4" s="18">
+        <v>1.44</v>
+      </c>
+      <c r="H4" s="19">
+        <v>1.81</v>
+      </c>
+      <c r="I4" s="19">
+        <v>1.88</v>
+      </c>
+      <c r="J4" s="19">
+        <v>1.93</v>
+      </c>
+      <c r="K4" s="20">
+        <v>2.35</v>
+      </c>
+      <c r="L4" s="20">
+        <v>2.4</v>
+      </c>
+      <c r="M4" s="20">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="N4" s="21">
+        <v>2.88</v>
+      </c>
+      <c r="O4" s="21">
+        <v>2.95</v>
+      </c>
+      <c r="P4" s="21">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="22">
+        <v>3.4</v>
+      </c>
+      <c r="R4" s="22">
+        <v>3.49</v>
+      </c>
+      <c r="S4" s="22">
+        <v>3.54</v>
+      </c>
+      <c r="T4" s="23">
+        <v>4.01</v>
+      </c>
+      <c r="U4" s="23">
+        <v>4.09</v>
+      </c>
+      <c r="V4" s="23">
+        <v>4.1500000000000004</v>
+      </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="B5" s="17">
+        <v>0.76</v>
+      </c>
+      <c r="C5" s="17">
+        <v>0.85</v>
+      </c>
+      <c r="D5" s="17">
+        <v>0.88</v>
+      </c>
+      <c r="E5" s="18">
+        <v>1.19</v>
+      </c>
+      <c r="F5" s="18">
+        <v>1.29</v>
+      </c>
+      <c r="G5" s="18">
+        <v>1.23</v>
+      </c>
+      <c r="H5" s="19">
+        <v>1.66</v>
+      </c>
+      <c r="I5" s="19">
+        <v>1.7</v>
+      </c>
+      <c r="J5" s="19">
+        <v>1.71</v>
+      </c>
+      <c r="K5" s="20">
+        <v>2.34</v>
+      </c>
+      <c r="L5" s="20">
+        <v>2.38</v>
+      </c>
+      <c r="M5" s="20">
+        <v>2.38</v>
+      </c>
+      <c r="N5" s="21">
+        <v>3.01</v>
+      </c>
+      <c r="O5" s="21">
+        <v>3.03</v>
+      </c>
+      <c r="P5" s="21">
+        <v>3.03</v>
+      </c>
+      <c r="Q5" s="22">
+        <v>3.65</v>
+      </c>
+      <c r="R5" s="22">
+        <v>3.68</v>
+      </c>
+      <c r="S5" s="22">
+        <v>3.68</v>
+      </c>
+      <c r="T5" s="23">
+        <v>4.2</v>
+      </c>
+      <c r="U5" s="23">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="V5" s="23">
+        <v>4.3600000000000003</v>
+      </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="6">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="C6" s="6">
-        <v>0.59</v>
-      </c>
-      <c r="D6" s="6">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="E6" s="6">
-        <v>0.96</v>
-      </c>
-      <c r="F6" s="6">
-        <v>1</v>
-      </c>
-      <c r="G6" s="6">
-        <v>0.98</v>
-      </c>
-      <c r="H6" s="6">
-        <v>1.29</v>
-      </c>
-      <c r="I6" s="6">
-        <v>1.31</v>
-      </c>
-      <c r="J6" s="6">
-        <v>1.31</v>
-      </c>
-      <c r="K6" s="6">
-        <v>1.8</v>
-      </c>
-      <c r="L6" s="6">
-        <v>1.8</v>
-      </c>
-      <c r="M6" s="6">
+      <c r="B6" s="17">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="C6" s="17">
+        <v>0.92</v>
+      </c>
+      <c r="D6" s="17">
+        <v>0.92</v>
+      </c>
+      <c r="E6" s="18">
+        <v>2.02</v>
+      </c>
+      <c r="F6" s="18">
         <v>1.76</v>
       </c>
-      <c r="N6" s="6">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="O6" s="6">
-        <v>2.31</v>
-      </c>
-      <c r="P6" s="6">
-        <v>2.29</v>
-      </c>
-      <c r="Q6" s="6">
-        <v>2.72</v>
-      </c>
-      <c r="R6" s="6">
-        <v>2.72</v>
-      </c>
-      <c r="S6" s="6">
-        <v>2.79</v>
-      </c>
-      <c r="T6" s="6">
-        <v>3.16</v>
-      </c>
-      <c r="U6" s="6">
-        <v>3.19</v>
-      </c>
-      <c r="V6" s="6">
-        <v>3.27</v>
+      <c r="G6" s="18">
+        <v>1.75</v>
+      </c>
+      <c r="H6" s="19">
+        <v>2.86</v>
+      </c>
+      <c r="I6" s="19">
+        <v>2.69</v>
+      </c>
+      <c r="J6" s="19">
+        <v>2.58</v>
+      </c>
+      <c r="K6" s="20">
+        <v>3.69</v>
+      </c>
+      <c r="L6" s="20">
+        <v>3.43</v>
+      </c>
+      <c r="M6" s="20">
+        <v>3.4</v>
+      </c>
+      <c r="N6" s="21">
+        <v>4.5</v>
+      </c>
+      <c r="O6" s="21">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="P6" s="21">
+        <v>4.21</v>
+      </c>
+      <c r="Q6" s="22">
+        <v>5.31</v>
+      </c>
+      <c r="R6" s="22">
+        <v>5.05</v>
+      </c>
+      <c r="S6" s="22">
+        <v>5.03</v>
+      </c>
+      <c r="T6" s="23">
+        <v>6.13</v>
+      </c>
+      <c r="U6" s="23">
+        <v>5.88</v>
+      </c>
+      <c r="V6" s="23">
+        <v>5.83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>